<commit_message>
[export] Display HoursWorked for exported warrants
</commit_message>
<xml_diff>
--- a/GrantCountyAS400/GrantCountyAs400.Web/wwwroot/ExcelTemplates/AccountPayrollTemplate.xlsx
+++ b/GrantCountyAS400/GrantCountyAs400.Web/wwwroot/ExcelTemplates/AccountPayrollTemplate.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF88233-ED38-4AEF-8C1A-DBF5AAA74F01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -51,12 +52,15 @@
   </si>
   <si>
     <t>Net Pay</t>
+  </si>
+  <si>
+    <t>Hours Worked</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
@@ -124,6 +128,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -171,7 +178,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,9 +211,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,6 +263,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -414,7 +455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -445,8 +486,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -456,9 +497,10 @@
     <col min="3" max="3" width="8.88671875" style="2"/>
     <col min="7" max="7" width="32.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -486,8 +528,11 @@
       <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Deferred gross and taxable to Excel template
</commit_message>
<xml_diff>
--- a/GrantCountyAS400/GrantCountyAs400.Web/wwwroot/ExcelTemplates/AccountPayrollTemplate.xlsx
+++ b/GrantCountyAS400/GrantCountyAs400.Web/wwwroot/ExcelTemplates/AccountPayrollTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF88233-ED38-4AEF-8C1A-DBF5AAA74F01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283EB763-964D-44B7-BFED-B1157D05B0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Hours Worked</t>
+  </si>
+  <si>
+    <t>Def Gross</t>
+  </si>
+  <si>
+    <t>Taxable</t>
   </si>
 </sst>
 </file>
@@ -460,14 +466,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -487,20 +493,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -531,8 +537,14 @@
       <c r="J1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>